<commit_message>
Login - Read and write data to excel
</commit_message>
<xml_diff>
--- a/RestAssuredAutomation/data/TestData.xlsx
+++ b/RestAssuredAutomation/data/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{56FE419E-AEDA-45F5-B96C-40E4D72BD1F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E3A09961-430E-45B9-B6CE-0F5FB24D68DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17064" windowHeight="7728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <t>palash@tryspeed.com</t>
   </si>
   <si>
-    <t>Open@123</t>
+    <t>Admin@123</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L3:L4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>